<commit_message>
Updated Project Plan #1
Ahir's first update to the project
</commit_message>
<xml_diff>
--- a/documents/DroidAssistedParking_ProjectPlan.xlsx
+++ b/documents/DroidAssistedParking_ProjectPlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IoT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahirc\Desktop\iot-projects\smart-parking\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t xml:space="preserve">Week </t>
   </si>
@@ -75,9 +75,6 @@
     <t>Explore image processing options</t>
   </si>
   <si>
-    <t>1) Does the drone follow you vertically? Let's say when you climb stairs, does it maintain the altitude?</t>
-  </si>
-  <si>
     <t>Figure out battery life between charge (estd. 20min)</t>
   </si>
   <si>
@@ -121,6 +118,15 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Approximately 15 mins. Does not allow for takeoff after dropping below ~30%</t>
+  </si>
+  <si>
+    <t>Drone does not follow vertically, continues at about its same height from a distance while on "leash" mode.</t>
   </si>
 </sst>
 </file>
@@ -489,21 +495,21 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.42578125" customWidth="1"/>
+    <col min="3" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -529,52 +535,95 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="9">
+        <v>42528</v>
+      </c>
+      <c r="F2" s="9">
+        <v>42530</v>
+      </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9">
+        <v>42529</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="9">
+        <v>42529</v>
+      </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>16</v>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="9">
+        <v>42529</v>
+      </c>
+      <c r="F5" s="9">
+        <v>42529</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="9">
         <v>42527</v>
@@ -583,20 +632,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="9">
         <v>42528</v>
@@ -605,18 +654,18 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
@@ -626,56 +675,56 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>24</v>
@@ -690,9 +739,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -721,22 +770,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>

</xml_diff>